<commit_message>
EPBDS-11473 added more test cases
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11473_AmbihousInputsMathedToReturnWarns.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11473_AmbihousInputsMathedToReturnWarns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\Bugz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EIS_Sources\OpenL\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34ACC042-8045-46B0-A9FC-4506D96A9F81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B9C6B8-810D-4FE2-99AF-24DE91951070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="0" windowWidth="27360" windowHeight="15090" xr2:uid="{1AB9C06A-0008-4A6D-B946-682D428BF3FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1AB9C06A-0008-4A6D-B946-682D428BF3FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Datatype MyDatatype</t>
   </si>
@@ -41,9 +41,6 @@
     <t>myCode</t>
   </si>
   <si>
-    <t>SmartRules MyDatatype myRules( String myCode, MyDatatype myObj)</t>
-  </si>
-  <si>
     <t>code</t>
   </si>
   <si>
@@ -63,6 +60,21 @@
   </si>
   <si>
     <t>vvv</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>SmartRules MyDatatype myRules( String myCode, MyDatatype myObj, Date foo)</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>bar</t>
   </si>
 </sst>
 </file>
@@ -415,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA9103A-B1AF-41CE-A260-36D8BF2F2928}">
-  <dimension ref="D9:E18"/>
+  <dimension ref="D9:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,46 +450,62 @@
     </row>
     <row r="11" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="E11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" t="s">
-        <v>7</v>
+    </row>
+    <row r="12" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16">
-        <v>100</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17">
-        <v>200</v>
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20">
         <v>300</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EPBDS-11473 managing token aliases which are belongs the the same objects
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11473_AmbihousInputsMathedToReturnWarns.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11473_AmbihousInputsMathedToReturnWarns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EIS_Sources\OpenL\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B9C6B8-810D-4FE2-99AF-24DE91951070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EC56F5-CD4A-4EF7-8174-EFC6041B18D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1AB9C06A-0008-4A6D-B946-682D428BF3FF}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Datatype MyDatatype</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>bar</t>
+  </si>
+  <si>
+    <t>SmartRules MyDatatype myRules2( MyDatatype myObj)</t>
   </si>
 </sst>
 </file>
@@ -111,7 +114,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -427,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA9103A-B1AF-41CE-A260-36D8BF2F2928}">
-  <dimension ref="D9:E20"/>
+  <dimension ref="D9:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D31" sqref="D31:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +513,48 @@
         <v>300</v>
       </c>
     </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35">
+        <v>300</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D31:E31"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>